<commit_message>
Trying to get my fileprocessor to create a hashmap, counting my Yes and No for each individual feature
</commit_message>
<xml_diff>
--- a/freqTable.xlsx
+++ b/freqTable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\b4n73\IdeaProjects\oopjava_mlproject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1204015C-A955-4DB1-A467-A2FA485408FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1806C8DB-9B14-47D9-8ABD-F6CCA23E98B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1972B8FF-4276-4FFE-9B23-D3E12F249647}"/>
+    <workbookView xWindow="4740" yWindow="3360" windowWidth="17280" windowHeight="8880" xr2:uid="{1972B8FF-4276-4FFE-9B23-D3E12F249647}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -468,6 +468,12 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.88671875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="C1" t="s">

</xml_diff>